<commit_message>
Adding coordonnees_gps_fosa field on each xls form linked to the Health facilities type
</commit_message>
<xml_diff>
--- a/setuper/data/entity-child_registration_2022090701.xlsx
+++ b/setuper/data/entity-child_registration_2022090701.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="105">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -133,6 +133,15 @@
   </si>
   <si>
     <t xml:space="preserve">${age_type} = 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">geopoint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coordonnees_gps_fosa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPS coordinates of the health facility</t>
   </si>
   <si>
     <t xml:space="preserve">child_details</t>
@@ -404,7 +413,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -414,7 +423,13 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFF6F9D4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF6F9D4"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -452,7 +467,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -485,6 +500,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -510,6 +529,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFF6F9D4"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -518,17 +597,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="35.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="40.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="82.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="42.43"/>
@@ -748,42 +827,35 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
+      <c r="A11" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="4"/>
       <c r="H11" s="4"/>
-    </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>39</v>
-      </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="C13" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="H13" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="6" t="s">
-        <v>20</v>
+      <c r="A14" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>44</v>
@@ -792,49 +864,62 @@
         <v>45</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="6" t="s">
         <v>51</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J16" s="4"/>
+        <v>46</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
         <v>52</v>
       </c>
+      <c r="B17" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J17" s="4"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1816,6 +1901,7 @@
     <row r="998" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="999" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1000" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1001" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1838,23 +1924,23 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B1" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -1880,13 +1966,13 @@
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B3" s="8" t="n">
+        <v>59</v>
+      </c>
+      <c r="B3" s="9" t="n">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -1913,13 +1999,13 @@
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B4" s="8" t="n">
+        <v>59</v>
+      </c>
+      <c r="B4" s="9" t="n">
         <v>0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -1946,102 +2032,102 @@
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2075,13 +2161,13 @@
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
@@ -2108,13 +2194,13 @@
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
@@ -2141,13 +2227,13 @@
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
@@ -2201,17 +2287,17 @@
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
@@ -2236,17 +2322,17 @@
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="4" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
@@ -2271,17 +2357,17 @@
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="4" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
@@ -2306,17 +2392,17 @@
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="4" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
@@ -2341,17 +2427,17 @@
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="4" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
@@ -2376,25 +2462,25 @@
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="B28" s="9" t="n">
+      <c r="A28" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B28" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="C28" s="9" t="s">
-        <v>96</v>
+      <c r="C28" s="10" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="B29" s="9" t="n">
+      <c r="A29" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B29" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="C29" s="9" t="s">
-        <v>97</v>
+      <c r="C29" s="10" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -3386,11 +3472,11 @@
   </sheetPr>
   <dimension ref="A1:U1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="55.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="77.52"/>
@@ -3398,11 +3484,11 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>99</v>
+      <c r="A1" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>102</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -3425,11 +3511,11 @@
       <c r="U1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>101</v>
+      <c r="A2" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>104</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>

</xml_diff>

<commit_message>
Update child registration form
</commit_message>
<xml_diff>
--- a/setuper/data/entity-child_registration_2022090701.xlsx
+++ b/setuper/data/entity-child_registration_2022090701.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="104">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -63,6 +63,9 @@
     <t xml:space="preserve">calculation</t>
   </si>
   <si>
+    <t xml:space="preserve">parameters</t>
+  </si>
+  <si>
     <t xml:space="preserve">start</t>
   </si>
   <si>
@@ -84,21 +87,51 @@
     <t xml:space="preserve">Registration</t>
   </si>
   <si>
+    <t xml:space="preserve">field-list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">geopoint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coordonnees_gps_fosa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPS coordinates</t>
+  </si>
+  <si>
     <t xml:space="preserve">text</t>
   </si>
   <si>
     <t xml:space="preserve">Child's Name</t>
   </si>
   <si>
-    <t xml:space="preserve">yes</t>
-  </si>
-  <si>
     <t xml:space="preserve">father_name</t>
   </si>
   <si>
     <t xml:space="preserve">Father Name</t>
   </si>
   <si>
+    <t xml:space="preserve">image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">picture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Take a picture of the child</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max-pixels=1000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_one gender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gender</t>
+  </si>
+  <si>
     <t xml:space="preserve">select_one cal_mo</t>
   </si>
   <si>
@@ -135,36 +168,6 @@
     <t xml:space="preserve">${age_type} = 0</t>
   </si>
   <si>
-    <t xml:space="preserve">geopoint</t>
-  </si>
-  <si>
-    <t xml:space="preserve">coordonnees_gps_fosa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPS coordinates of the health facility</t>
-  </si>
-  <si>
-    <t xml:space="preserve">child_details</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Child Details</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${age} &lt; 59 or round((today() - ${birth_date}) div 12) &lt; 59</t>
-  </si>
-  <si>
-    <t xml:space="preserve">select_one gender</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gender</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gender</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no</t>
-  </si>
-  <si>
     <t xml:space="preserve">caretaker_name</t>
   </si>
   <si>
@@ -180,112 +183,106 @@
     <t xml:space="preserve">Relationship with child</t>
   </si>
   <si>
-    <t xml:space="preserve">select_one hc</t>
+    <t xml:space="preserve">end group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">list name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">village</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes_no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">male</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Male</t>
+  </si>
+  <si>
+    <t xml:space="preserve">female</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Female</t>
+  </si>
+  <si>
+    <t xml:space="preserve">caretaker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mother</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mother</t>
+  </si>
+  <si>
+    <t xml:space="preserve">father</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Father</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sister</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sister</t>
+  </si>
+  <si>
+    <t xml:space="preserve">brother</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brother</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grandfather</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grandfather</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grandmother</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grandmother</t>
+  </si>
+  <si>
+    <t xml:space="preserve">other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">villages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">village_A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Village A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">village_B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Village B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">village_C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Village C</t>
   </si>
   <si>
     <t xml:space="preserve">hc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Health Center</t>
-  </si>
-  <si>
-    <t xml:space="preserve">end group</t>
-  </si>
-  <si>
-    <t xml:space="preserve">list name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">village</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes_no</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No</t>
-  </si>
-  <si>
-    <t xml:space="preserve">male</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Male</t>
-  </si>
-  <si>
-    <t xml:space="preserve">female</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Female</t>
-  </si>
-  <si>
-    <t xml:space="preserve">caretaker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mother</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mother</t>
-  </si>
-  <si>
-    <t xml:space="preserve">father</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Father</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sister</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sister</t>
-  </si>
-  <si>
-    <t xml:space="preserve">brother</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brother</t>
-  </si>
-  <si>
-    <t xml:space="preserve">grandfather</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grandfather</t>
-  </si>
-  <si>
-    <t xml:space="preserve">grandmother</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grandmother</t>
-  </si>
-  <si>
-    <t xml:space="preserve">other</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other</t>
-  </si>
-  <si>
-    <t xml:space="preserve">villages</t>
-  </si>
-  <si>
-    <t xml:space="preserve">village_A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Village A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">village_B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Village B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">village_C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Village C</t>
   </si>
   <si>
     <t xml:space="preserve">hc_A</t>
@@ -346,7 +343,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -391,6 +388,13 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Helvetica Neue"/>
@@ -413,7 +417,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -422,14 +426,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFF6F9D4"/>
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF6F9D4"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFF6F9D4"/>
       </patternFill>
     </fill>
   </fills>
@@ -467,7 +477,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -484,23 +494,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -508,16 +518,12 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -597,20 +603,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z1001"/>
+  <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="40.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="82.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="42.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="40.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="42.44"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -653,7 +659,9 @@
       <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1"/>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
@@ -669,13 +677,13 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -703,13 +711,13 @@
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -736,190 +744,150 @@
       <c r="Z3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" s="4" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="4" t="s">
+      <c r="A6" s="5" t="s">
         <v>22</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>22</v>
+      <c r="A7" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="6" t="s">
+      <c r="B8" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>22</v>
+      <c r="C8" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="4" t="s">
+      <c r="A9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="B9" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H9" s="4" t="s">
+      <c r="C9" s="1" t="s">
         <v>31</v>
+      </c>
+      <c r="N9" s="7" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="4" t="s">
+      <c r="A10" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="B10" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="4" t="s">
+      <c r="C10" s="0" t="s">
         <v>35</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="C11" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="8" t="s">
+    </row>
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="4"/>
-      <c r="H11" s="4"/>
+      <c r="B12" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>42</v>
+      <c r="A13" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>46</v>
+      <c r="A14" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>46</v>
+      <c r="A15" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>52</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" s="4" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J17" s="4"/>
-    </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1899,9 +1867,6 @@
     <row r="996" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="997" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="998" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="999" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1000" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1001" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1920,15 +1885,15 @@
   </sheetPr>
   <dimension ref="A1:Y1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>1</v>
@@ -1937,10 +1902,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -1966,13 +1931,13 @@
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B3" s="9" t="n">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -1999,13 +1964,13 @@
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B4" s="9" t="n">
         <v>0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -2031,103 +1996,103 @@
       <c r="Y4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>63</v>
+      <c r="A5" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>65</v>
+      <c r="A6" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="0" t="s">
         <v>66</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>70</v>
+      <c r="A9" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>72</v>
+      <c r="A10" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>74</v>
+      <c r="A11" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>76</v>
+      <c r="A12" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>78</v>
+      <c r="A13" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>80</v>
+      <c r="A14" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2138,349 +2103,132 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
-      <c r="P17" s="4"/>
-      <c r="Q17" s="4"/>
-      <c r="R17" s="4"/>
-      <c r="S17" s="4"/>
-      <c r="T17" s="4"/>
-      <c r="U17" s="4"/>
-      <c r="V17" s="4"/>
-      <c r="W17" s="4"/>
-      <c r="X17" s="4"/>
-      <c r="Y17" s="4"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
-      <c r="O18" s="4"/>
-      <c r="P18" s="4"/>
-      <c r="Q18" s="4"/>
-      <c r="R18" s="4"/>
-      <c r="S18" s="4"/>
-      <c r="T18" s="4"/>
-      <c r="U18" s="4"/>
-      <c r="V18" s="4"/>
-      <c r="W18" s="4"/>
-      <c r="X18" s="4"/>
-      <c r="Y18" s="4"/>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
-      <c r="O19" s="4"/>
-      <c r="P19" s="4"/>
-      <c r="Q19" s="4"/>
-      <c r="R19" s="4"/>
-      <c r="S19" s="4"/>
-      <c r="T19" s="4"/>
-      <c r="U19" s="4"/>
-      <c r="V19" s="4"/>
-      <c r="W19" s="4"/>
-      <c r="X19" s="4"/>
-      <c r="Y19" s="4"/>
+        <v>83</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="B22" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="4"/>
-      <c r="P20" s="4"/>
-      <c r="Q20" s="4"/>
-      <c r="R20" s="4"/>
-      <c r="S20" s="4"/>
-      <c r="T20" s="4"/>
-      <c r="U20" s="4"/>
-      <c r="V20" s="4"/>
-      <c r="W20" s="4"/>
-      <c r="X20" s="4"/>
-      <c r="Y20" s="4"/>
-    </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
-      <c r="N21" s="4"/>
-      <c r="O21" s="4"/>
-      <c r="P21" s="4"/>
-      <c r="Q21" s="4"/>
-      <c r="R21" s="4"/>
-      <c r="S21" s="4"/>
-      <c r="T21" s="4"/>
-      <c r="U21" s="4"/>
-      <c r="V21" s="4"/>
-      <c r="W21" s="4"/>
-      <c r="X21" s="4"/>
-      <c r="Y21" s="4"/>
-    </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B22" s="4" t="s">
+      <c r="C22" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
-      <c r="N22" s="4"/>
-      <c r="O22" s="4"/>
-      <c r="P22" s="4"/>
-      <c r="Q22" s="4"/>
-      <c r="R22" s="4"/>
-      <c r="S22" s="4"/>
-      <c r="T22" s="4"/>
-      <c r="U22" s="4"/>
-      <c r="V22" s="4"/>
-      <c r="W22" s="4"/>
-      <c r="X22" s="4"/>
-      <c r="Y22" s="4"/>
+      <c r="E22" s="0" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B23" s="4" t="s">
+      <c r="A23" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="C23" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
-      <c r="M23" s="4"/>
-      <c r="N23" s="4"/>
-      <c r="O23" s="4"/>
-      <c r="P23" s="4"/>
-      <c r="Q23" s="4"/>
-      <c r="R23" s="4"/>
-      <c r="S23" s="4"/>
-      <c r="T23" s="4"/>
-      <c r="U23" s="4"/>
-      <c r="V23" s="4"/>
-      <c r="W23" s="4"/>
-      <c r="X23" s="4"/>
-      <c r="Y23" s="4"/>
+      <c r="E23" s="0" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B24" s="4" t="s">
+      <c r="A24" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C24" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
-      <c r="M24" s="4"/>
-      <c r="N24" s="4"/>
-      <c r="O24" s="4"/>
-      <c r="P24" s="4"/>
-      <c r="Q24" s="4"/>
-      <c r="R24" s="4"/>
-      <c r="S24" s="4"/>
-      <c r="T24" s="4"/>
-      <c r="U24" s="4"/>
-      <c r="V24" s="4"/>
-      <c r="W24" s="4"/>
-      <c r="X24" s="4"/>
-      <c r="Y24" s="4"/>
+      <c r="E24" s="0" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B25" s="4" t="s">
+      <c r="A25" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="C25" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="C25" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
-      <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
-      <c r="L25" s="4"/>
-      <c r="M25" s="4"/>
-      <c r="N25" s="4"/>
-      <c r="O25" s="4"/>
-      <c r="P25" s="4"/>
-      <c r="Q25" s="4"/>
-      <c r="R25" s="4"/>
-      <c r="S25" s="4"/>
-      <c r="T25" s="4"/>
-      <c r="U25" s="4"/>
-      <c r="V25" s="4"/>
-      <c r="W25" s="4"/>
-      <c r="X25" s="4"/>
-      <c r="Y25" s="4"/>
+      <c r="E25" s="0" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B26" s="4" t="s">
+      <c r="A26" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="C26" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="C26" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
-      <c r="N26" s="4"/>
-      <c r="O26" s="4"/>
-      <c r="P26" s="4"/>
-      <c r="Q26" s="4"/>
-      <c r="R26" s="4"/>
-      <c r="S26" s="4"/>
-      <c r="T26" s="4"/>
-      <c r="U26" s="4"/>
-      <c r="V26" s="4"/>
-      <c r="W26" s="4"/>
-      <c r="X26" s="4"/>
-      <c r="Y26" s="4"/>
+      <c r="E26" s="0" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B28" s="10" t="n">
         <v>1</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B29" s="10" t="n">
         <v>0</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -3476,19 +3224,19 @@
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="55.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="77.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="55.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="77.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.45"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>101</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>102</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -3511,11 +3259,11 @@
       <c r="U1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>103</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>104</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -3587,29 +3335,7 @@
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="4"/>
-      <c r="R9" s="4"/>
-      <c r="S9" s="4"/>
-      <c r="T9" s="4"/>
-      <c r="U9" s="4"/>
-    </row>
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>